<commit_message>
Mappings for non-AD invoices
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Invoice.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Invoice.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{739DA518-C2F0-4345-B2DE-683BDE515795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{584E9A8C-5CF8-4D4F-BB69-538DC931A551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26840" yWindow="6340" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="4" r:id="rId1"/>
     <sheet name="finance_invoice_ad" sheetId="1" r:id="rId2"/>
-    <sheet name="inv_supervision_level_lookup" sheetId="2" r:id="rId3"/>
+    <sheet name="finance_invoice_non_ad" sheetId="5" r:id="rId3"/>
+    <sheet name="inv_supervision_level_lookup" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="83">
   <si>
     <t>table_name</t>
   </si>
@@ -257,6 +258,22 @@
   </si>
   <si>
     <t>Elizabeth advised this should be left blank/null</t>
+  </si>
+  <si>
+    <t>finance_invoice_non_ad</t>
+  </si>
+  <si>
+    <t>first_x_chars = {"col": "Invoice No", "result_col": "Invoice_Type", "num": 2}
+exclude_values = {"col": "Invoice_Type", "values": ["AD"]}</t>
+  </si>
+  <si>
+    <t>AD</t>
+  </si>
+  <si>
+    <t>start_of_tax_year</t>
+  </si>
+  <si>
+    <t>end_of_tax_year</t>
   </si>
 </sst>
 </file>
@@ -277,21 +294,25 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -604,7 +625,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -665,6 +686,29 @@
         <v>56</v>
       </c>
     </row>
+    <row r="3" spans="1:8" s="9" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+      <c r="A3" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="G7" s="14"/>
     </row>
@@ -677,9 +721,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P15" sqref="P15"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -848,14 +892,8 @@
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
-      <c r="H5" t="s">
-        <v>55</v>
-      </c>
-      <c r="J5" t="s">
-        <v>59</v>
-      </c>
-      <c r="K5" t="s">
-        <v>58</v>
+      <c r="M5" s="14" t="s">
+        <v>80</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="13" t="s">
@@ -2550,6 +2588,1885 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B46E64-4858-2243-9F40-616107ECC251}">
+  <dimension ref="A1:P1000"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="2" width="19.5" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
+    <col min="7" max="7" width="10.5" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="25.33203125" customWidth="1"/>
+    <col min="10" max="10" width="20" customWidth="1"/>
+    <col min="11" max="11" width="22.5" customWidth="1"/>
+    <col min="12" max="12" width="21.33203125" customWidth="1"/>
+    <col min="13" max="13" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="11.5" customWidth="1"/>
+    <col min="16" max="16" width="32.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="15" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="14" x14ac:dyDescent="0.15">
+      <c r="A2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="9"/>
+      <c r="O2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="O3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="N4" s="2"/>
+      <c r="O4" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="P4" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" t="s">
+        <v>59</v>
+      </c>
+      <c r="K5" t="s">
+        <v>58</v>
+      </c>
+      <c r="N5" s="2"/>
+      <c r="O5" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I6" s="11"/>
+      <c r="J6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="O6" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="M7" s="2"/>
+      <c r="O7" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" s="11"/>
+      <c r="J8" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="K8" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="L8" s="2"/>
+      <c r="O8" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" t="s">
+        <v>55</v>
+      </c>
+      <c r="J9" t="s">
+        <v>61</v>
+      </c>
+      <c r="K9" t="s">
+        <v>62</v>
+      </c>
+      <c r="O9" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="O10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="P10" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="O11" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="P11" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="O12" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="P12" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="O13" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="P13" s="14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" t="s">
+        <v>55</v>
+      </c>
+      <c r="J14" t="s">
+        <v>60</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="M15" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="O15" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="14" x14ac:dyDescent="0.15">
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B24" s="3"/>
+    </row>
+    <row r="25" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B27" s="3"/>
+    </row>
+    <row r="28" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B28" s="3"/>
+    </row>
+    <row r="29" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B29" s="3"/>
+    </row>
+    <row r="30" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B30" s="3"/>
+    </row>
+    <row r="31" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B32" s="3"/>
+    </row>
+    <row r="33" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B33" s="3"/>
+    </row>
+    <row r="34" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B34" s="3"/>
+    </row>
+    <row r="35" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B35" s="3"/>
+    </row>
+    <row r="36" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B36" s="3"/>
+    </row>
+    <row r="37" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B37" s="3"/>
+    </row>
+    <row r="38" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B38" s="3"/>
+    </row>
+    <row r="39" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B39" s="3"/>
+    </row>
+    <row r="40" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B40" s="3"/>
+    </row>
+    <row r="41" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B41" s="3"/>
+    </row>
+    <row r="42" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B42" s="3"/>
+    </row>
+    <row r="43" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B43" s="3"/>
+    </row>
+    <row r="44" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B44" s="3"/>
+    </row>
+    <row r="45" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B45" s="3"/>
+    </row>
+    <row r="46" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B46" s="3"/>
+    </row>
+    <row r="47" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B47" s="3"/>
+    </row>
+    <row r="48" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B48" s="3"/>
+    </row>
+    <row r="49" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B49" s="3"/>
+    </row>
+    <row r="50" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B50" s="3"/>
+    </row>
+    <row r="51" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B51" s="3"/>
+    </row>
+    <row r="52" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B52" s="3"/>
+    </row>
+    <row r="53" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B53" s="3"/>
+    </row>
+    <row r="54" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B54" s="3"/>
+    </row>
+    <row r="55" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B55" s="3"/>
+    </row>
+    <row r="56" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B56" s="3"/>
+    </row>
+    <row r="57" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B57" s="3"/>
+    </row>
+    <row r="58" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B58" s="3"/>
+    </row>
+    <row r="59" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B59" s="3"/>
+    </row>
+    <row r="60" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B60" s="3"/>
+    </row>
+    <row r="61" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B61" s="3"/>
+    </row>
+    <row r="62" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B62" s="3"/>
+    </row>
+    <row r="63" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B63" s="3"/>
+    </row>
+    <row r="64" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B64" s="3"/>
+    </row>
+    <row r="65" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B65" s="3"/>
+    </row>
+    <row r="66" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B66" s="3"/>
+    </row>
+    <row r="67" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B67" s="3"/>
+    </row>
+    <row r="68" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B68" s="3"/>
+    </row>
+    <row r="69" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B69" s="3"/>
+    </row>
+    <row r="70" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B70" s="3"/>
+    </row>
+    <row r="71" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B71" s="3"/>
+    </row>
+    <row r="72" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B72" s="3"/>
+    </row>
+    <row r="73" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B73" s="3"/>
+    </row>
+    <row r="74" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B74" s="3"/>
+    </row>
+    <row r="75" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B75" s="3"/>
+    </row>
+    <row r="76" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B76" s="3"/>
+    </row>
+    <row r="77" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B77" s="3"/>
+    </row>
+    <row r="78" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B78" s="3"/>
+    </row>
+    <row r="79" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B79" s="3"/>
+    </row>
+    <row r="80" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B80" s="3"/>
+    </row>
+    <row r="81" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B81" s="3"/>
+    </row>
+    <row r="82" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B82" s="3"/>
+    </row>
+    <row r="83" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B83" s="3"/>
+    </row>
+    <row r="84" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B84" s="3"/>
+    </row>
+    <row r="85" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B85" s="3"/>
+    </row>
+    <row r="86" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B86" s="3"/>
+    </row>
+    <row r="87" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B87" s="3"/>
+    </row>
+    <row r="88" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B88" s="3"/>
+    </row>
+    <row r="89" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B89" s="3"/>
+    </row>
+    <row r="90" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B90" s="3"/>
+    </row>
+    <row r="91" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B91" s="3"/>
+    </row>
+    <row r="92" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B92" s="3"/>
+    </row>
+    <row r="93" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B93" s="3"/>
+    </row>
+    <row r="94" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B94" s="3"/>
+    </row>
+    <row r="95" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B95" s="3"/>
+    </row>
+    <row r="96" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B96" s="3"/>
+    </row>
+    <row r="97" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B97" s="3"/>
+    </row>
+    <row r="98" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B98" s="3"/>
+    </row>
+    <row r="99" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B99" s="3"/>
+    </row>
+    <row r="100" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B100" s="3"/>
+    </row>
+    <row r="101" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B101" s="3"/>
+    </row>
+    <row r="102" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B102" s="3"/>
+    </row>
+    <row r="103" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B103" s="3"/>
+    </row>
+    <row r="104" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B104" s="3"/>
+    </row>
+    <row r="105" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B105" s="3"/>
+    </row>
+    <row r="106" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B106" s="3"/>
+    </row>
+    <row r="107" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B107" s="3"/>
+    </row>
+    <row r="108" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B108" s="3"/>
+    </row>
+    <row r="109" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B109" s="3"/>
+    </row>
+    <row r="110" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B110" s="3"/>
+    </row>
+    <row r="111" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B111" s="3"/>
+    </row>
+    <row r="112" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B112" s="3"/>
+    </row>
+    <row r="113" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B113" s="3"/>
+    </row>
+    <row r="114" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B114" s="3"/>
+    </row>
+    <row r="115" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B115" s="3"/>
+    </row>
+    <row r="116" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B116" s="3"/>
+    </row>
+    <row r="117" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B117" s="3"/>
+    </row>
+    <row r="118" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B118" s="3"/>
+    </row>
+    <row r="119" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B119" s="3"/>
+    </row>
+    <row r="120" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B120" s="3"/>
+    </row>
+    <row r="121" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B121" s="3"/>
+    </row>
+    <row r="122" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B122" s="3"/>
+    </row>
+    <row r="123" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B123" s="3"/>
+    </row>
+    <row r="124" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B124" s="3"/>
+    </row>
+    <row r="125" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B125" s="3"/>
+    </row>
+    <row r="126" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B126" s="3"/>
+    </row>
+    <row r="127" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B127" s="3"/>
+    </row>
+    <row r="128" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B128" s="3"/>
+    </row>
+    <row r="129" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B129" s="3"/>
+    </row>
+    <row r="130" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B130" s="3"/>
+    </row>
+    <row r="131" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B131" s="3"/>
+    </row>
+    <row r="132" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B132" s="3"/>
+    </row>
+    <row r="133" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B133" s="3"/>
+    </row>
+    <row r="134" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B134" s="3"/>
+    </row>
+    <row r="135" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B135" s="3"/>
+    </row>
+    <row r="136" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B136" s="3"/>
+    </row>
+    <row r="137" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B137" s="3"/>
+    </row>
+    <row r="138" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B138" s="3"/>
+    </row>
+    <row r="139" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B139" s="3"/>
+    </row>
+    <row r="140" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B140" s="3"/>
+    </row>
+    <row r="141" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B141" s="3"/>
+    </row>
+    <row r="142" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B142" s="3"/>
+    </row>
+    <row r="143" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B143" s="3"/>
+    </row>
+    <row r="144" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B144" s="3"/>
+    </row>
+    <row r="145" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B145" s="3"/>
+    </row>
+    <row r="146" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B146" s="3"/>
+    </row>
+    <row r="147" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B147" s="3"/>
+    </row>
+    <row r="148" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B148" s="3"/>
+    </row>
+    <row r="149" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B149" s="3"/>
+    </row>
+    <row r="150" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B150" s="3"/>
+    </row>
+    <row r="151" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B151" s="3"/>
+    </row>
+    <row r="152" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B152" s="3"/>
+    </row>
+    <row r="153" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B153" s="3"/>
+    </row>
+    <row r="154" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B154" s="3"/>
+    </row>
+    <row r="155" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B155" s="3"/>
+    </row>
+    <row r="156" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B156" s="3"/>
+    </row>
+    <row r="157" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B157" s="3"/>
+    </row>
+    <row r="158" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B158" s="3"/>
+    </row>
+    <row r="159" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B159" s="3"/>
+    </row>
+    <row r="160" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B160" s="3"/>
+    </row>
+    <row r="161" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B161" s="3"/>
+    </row>
+    <row r="162" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B162" s="3"/>
+    </row>
+    <row r="163" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B163" s="3"/>
+    </row>
+    <row r="164" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B164" s="3"/>
+    </row>
+    <row r="165" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B165" s="3"/>
+    </row>
+    <row r="166" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B166" s="3"/>
+    </row>
+    <row r="167" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B167" s="3"/>
+    </row>
+    <row r="168" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B168" s="3"/>
+    </row>
+    <row r="169" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B169" s="3"/>
+    </row>
+    <row r="170" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B170" s="3"/>
+    </row>
+    <row r="171" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B171" s="3"/>
+    </row>
+    <row r="172" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B172" s="3"/>
+    </row>
+    <row r="173" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B173" s="3"/>
+    </row>
+    <row r="174" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B174" s="3"/>
+    </row>
+    <row r="175" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B175" s="3"/>
+    </row>
+    <row r="176" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B176" s="3"/>
+    </row>
+    <row r="177" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B177" s="3"/>
+    </row>
+    <row r="178" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B178" s="3"/>
+    </row>
+    <row r="179" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B179" s="3"/>
+    </row>
+    <row r="180" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B180" s="3"/>
+    </row>
+    <row r="181" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B181" s="3"/>
+    </row>
+    <row r="182" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B182" s="3"/>
+    </row>
+    <row r="183" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B183" s="3"/>
+    </row>
+    <row r="184" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B184" s="3"/>
+    </row>
+    <row r="185" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B185" s="3"/>
+    </row>
+    <row r="186" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B186" s="3"/>
+    </row>
+    <row r="187" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B187" s="3"/>
+    </row>
+    <row r="188" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B188" s="3"/>
+    </row>
+    <row r="189" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B189" s="3"/>
+    </row>
+    <row r="190" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B190" s="3"/>
+    </row>
+    <row r="191" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B191" s="3"/>
+    </row>
+    <row r="192" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B192" s="3"/>
+    </row>
+    <row r="193" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B193" s="3"/>
+    </row>
+    <row r="194" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B194" s="3"/>
+    </row>
+    <row r="195" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B195" s="3"/>
+    </row>
+    <row r="196" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B196" s="3"/>
+    </row>
+    <row r="197" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B197" s="3"/>
+    </row>
+    <row r="198" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B198" s="3"/>
+    </row>
+    <row r="199" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B199" s="3"/>
+    </row>
+    <row r="200" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B200" s="3"/>
+    </row>
+    <row r="201" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B201" s="3"/>
+    </row>
+    <row r="202" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B202" s="3"/>
+    </row>
+    <row r="203" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B203" s="3"/>
+    </row>
+    <row r="204" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B204" s="3"/>
+    </row>
+    <row r="205" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B205" s="3"/>
+    </row>
+    <row r="206" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B206" s="3"/>
+    </row>
+    <row r="207" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B207" s="3"/>
+    </row>
+    <row r="208" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B208" s="3"/>
+    </row>
+    <row r="209" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B209" s="3"/>
+    </row>
+    <row r="210" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B210" s="3"/>
+    </row>
+    <row r="211" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B211" s="3"/>
+    </row>
+    <row r="212" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B212" s="3"/>
+    </row>
+    <row r="213" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B213" s="3"/>
+    </row>
+    <row r="214" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B214" s="3"/>
+    </row>
+    <row r="215" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B215" s="3"/>
+    </row>
+    <row r="216" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B216" s="3"/>
+    </row>
+    <row r="217" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B217" s="3"/>
+    </row>
+    <row r="218" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B218" s="3"/>
+    </row>
+    <row r="219" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B219" s="3"/>
+    </row>
+    <row r="220" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B220" s="3"/>
+    </row>
+    <row r="221" spans="2:2" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="222" spans="2:2" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="223" spans="2:2" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="224" spans="2:2" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="225" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="226" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="227" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="228" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="229" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="230" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="231" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="232" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="233" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="234" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="235" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="236" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="237" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="238" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="239" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="240" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="241" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="242" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="243" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="244" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="245" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="246" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="247" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="248" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="249" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="250" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="251" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="252" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="253" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="254" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="255" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="256" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="257" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="258" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="259" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="260" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="261" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="262" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="263" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="264" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="265" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="266" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="267" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="268" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="269" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="270" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="271" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="272" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="273" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="274" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="275" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="276" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="277" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="278" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="279" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="280" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="281" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="282" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="283" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="284" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="285" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="286" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="287" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="288" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="289" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="290" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="291" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="292" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="293" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="294" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="295" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="296" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="297" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="298" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="299" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="300" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="301" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="302" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="303" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="304" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="305" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="306" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="307" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="308" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="309" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="310" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="311" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="312" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="313" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="314" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="315" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="316" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="317" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="318" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="319" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="320" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="321" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="322" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="323" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="324" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="325" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="326" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="327" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="328" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="329" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="330" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="331" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="332" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="333" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="334" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="335" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="336" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="337" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="338" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="339" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="340" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="341" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="342" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="343" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="344" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="345" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="346" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="347" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="348" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="349" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="350" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="351" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="352" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="353" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="354" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="355" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="356" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="357" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="358" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="359" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="360" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="361" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="362" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="363" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="364" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="365" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="366" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="367" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="368" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="369" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="370" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="371" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="372" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="373" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="374" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="375" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="376" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="377" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="378" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="379" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="380" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="381" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="382" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="383" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="384" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="385" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="386" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="387" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="388" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="389" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="390" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="391" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="392" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="393" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="394" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="395" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="396" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="397" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="398" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="399" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="400" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="401" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="402" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="403" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="404" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="405" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="406" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="407" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="408" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="409" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="410" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="411" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="412" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="413" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="414" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="415" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="416" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="417" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="418" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="419" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="420" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="421" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="422" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="423" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="424" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="425" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="426" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="427" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="428" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="429" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="430" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="431" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="432" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="433" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="434" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="435" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="436" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="437" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="438" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="439" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="440" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="441" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="442" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="443" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="444" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="445" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="446" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="447" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="448" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="449" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="450" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="451" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="452" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="453" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="454" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="455" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="456" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="457" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="458" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="459" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="460" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="461" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="462" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="463" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="464" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="465" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="466" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="467" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="468" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="469" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="470" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="471" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="472" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="473" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="474" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="475" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="476" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="477" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="478" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="479" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="480" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="481" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="482" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="483" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="484" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="485" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="486" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="487" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="488" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="489" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="490" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="491" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="492" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="493" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="494" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="495" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="496" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="497" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="498" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="499" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="500" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="501" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="502" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="503" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="504" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="505" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="506" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="507" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="508" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="509" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="510" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="511" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="512" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="513" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="514" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="515" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="516" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="517" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="518" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="519" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="520" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="521" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="522" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="523" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="524" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="525" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="526" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="527" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="528" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="529" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="530" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="531" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="532" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="533" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="534" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="535" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="536" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="537" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="538" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="539" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="540" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="541" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="542" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="543" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="544" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="545" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="546" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="547" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="548" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="549" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="550" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="551" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="552" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="553" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="554" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="555" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="556" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="557" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="558" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="559" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="560" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="561" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="562" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="563" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="564" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="565" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="566" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="567" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="568" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="569" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="570" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="571" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="572" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="573" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="574" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="575" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="576" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="577" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="578" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="579" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="580" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="581" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="582" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="583" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="584" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="585" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="586" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="587" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="588" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="589" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="590" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="591" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="592" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="593" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="594" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="595" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="596" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="597" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="598" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="599" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="600" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="601" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="602" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="603" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="604" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="605" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="606" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="607" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="608" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="609" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="610" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="611" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="612" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="613" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="614" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="615" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="616" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="617" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="618" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="619" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="620" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="621" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="622" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="623" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="624" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="625" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="626" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="627" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="628" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="629" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="630" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="631" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="632" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="633" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="634" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="635" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="636" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="637" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="638" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="639" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="640" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="641" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="642" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="643" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="644" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="645" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="646" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="647" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="648" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="649" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="650" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="651" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="652" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="653" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="654" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="655" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="656" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="657" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="658" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="659" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="660" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="661" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="662" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="663" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="664" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="665" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="666" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="667" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="668" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="669" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="670" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="671" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="672" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="673" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="674" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="675" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="676" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="677" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="678" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="679" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="680" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="681" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="682" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="683" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="684" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="685" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="686" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="687" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="688" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="689" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="690" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="691" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="692" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="693" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="694" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="695" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="696" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="697" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="698" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="699" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="700" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="701" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="702" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="703" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="704" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="705" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="706" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="707" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="708" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="709" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="710" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="711" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="712" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="713" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="714" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="715" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="716" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="717" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="718" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="719" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="720" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="721" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="722" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="723" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="724" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="725" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="726" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="727" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="728" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="729" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="730" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="731" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="732" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="733" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="734" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="735" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="736" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="737" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="738" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="739" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="740" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="741" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="742" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="743" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="744" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="745" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="746" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="747" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="748" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="749" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="750" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="751" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="752" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="753" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="754" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="755" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="756" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="757" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="758" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="759" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="760" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="761" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="762" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="763" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="764" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="765" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="766" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="767" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="768" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="769" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="770" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="771" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="772" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="773" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="774" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="775" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="776" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="777" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="778" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="779" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="780" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="781" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="782" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="783" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="784" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="785" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="786" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="787" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="788" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="789" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="790" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="791" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="792" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="793" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="794" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="795" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="796" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="797" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="798" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="799" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="800" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="801" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="802" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="803" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="804" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="805" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="806" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="807" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="808" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="809" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="810" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="811" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="812" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="813" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="814" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="815" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="816" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="817" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="818" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="819" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="820" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="821" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="822" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="823" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="824" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="825" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="826" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="827" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="828" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="829" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="830" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="831" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="832" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="833" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="834" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="835" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="836" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="837" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="838" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="839" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="840" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="841" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="842" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="843" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="844" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="845" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="846" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="847" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="848" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="849" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="850" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="851" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="852" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="853" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="854" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="855" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="856" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="857" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="858" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="859" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="860" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="861" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="862" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="863" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="864" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="865" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="866" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="867" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="868" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="869" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="870" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="871" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="872" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="873" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="874" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="875" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="876" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="877" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="878" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="879" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="880" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="881" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="882" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="883" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="884" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="885" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="886" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="887" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="888" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="889" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="890" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="891" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="892" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="893" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="894" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="895" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="896" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="897" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="898" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="899" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="900" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="901" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="902" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="903" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="904" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="905" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="906" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="907" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="908" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="909" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="910" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="911" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="912" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="913" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="914" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="915" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="916" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="917" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="918" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="919" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="920" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="921" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="922" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="923" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="924" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="925" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="926" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="927" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="928" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="929" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="930" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="931" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="932" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="933" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="934" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="935" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="936" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="937" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="938" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="939" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="940" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="941" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="942" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="943" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="944" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="945" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="946" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="947" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="948" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="949" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="950" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="951" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="952" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="953" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="954" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="955" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="956" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="957" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="958" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="959" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="960" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="961" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="962" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="963" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="964" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="965" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="966" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="967" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="968" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="969" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="970" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="971" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="972" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="973" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="974" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="975" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="976" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="977" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="978" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="979" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="980" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="981" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="982" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="983" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="984" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="985" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="986" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="987" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="988" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="989" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="990" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="991" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="992" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="993" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="994" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="995" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="996" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="997" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="998" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="999" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="1000" ht="13" x14ac:dyDescent="0.15"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup orientation="landscape"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>

<commit_message>
IN-882 Add conditionals for filtering out old Closed invoices, while also excluding credits from feeeexport
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Invoice.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Invoice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{584E9A8C-5CF8-4D4F-BB69-538DC931A551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A81D008-99FB-8F42-B828-D7BF45CF8294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35200" yWindow="6220" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="81">
   <si>
     <t>table_name</t>
   </si>
@@ -88,9 +88,6 @@
     <t>date</t>
   </si>
   <si>
-    <t>NO</t>
-  </si>
-  <si>
     <t>supervisionlevel</t>
   </si>
   <si>
@@ -193,9 +190,6 @@
     <t>feeexport</t>
   </si>
   <si>
-    <t>Case, Invoice No</t>
-  </si>
-  <si>
     <t>Person ID set in persons table</t>
   </si>
   <si>
@@ -235,9 +229,6 @@
     <t>CASRECMIGRATION</t>
   </si>
   <si>
-    <t>Populated at integration stage</t>
-  </si>
-  <si>
     <t>finance_invoice_ad</t>
   </si>
   <si>
@@ -247,33 +238,40 @@
     <t>GL Date from feecheck, populated from feecheck joined table</t>
   </si>
   <si>
+    <t>Elizabeth advised this should be left blank/null</t>
+  </si>
+  <si>
+    <t>finance_invoice_non_ad</t>
+  </si>
+  <si>
+    <t>AD</t>
+  </si>
+  <si>
+    <t>start_of_tax_year</t>
+  </si>
+  <si>
+    <t>end_of_tax_year</t>
+  </si>
+  <si>
+    <t>Populated via post-migration task</t>
+  </si>
+  <si>
+    <t>Linked to existing Finance Person via post-migration task</t>
+  </si>
+  <si>
     <t>first_x_chars = {"col": "Invoice No", "result_col": "Invoice_Type", "num": 2}
-Invoice_Type = "AD"</t>
-  </si>
-  <si>
-    <t>Map to existing id from finance_person table</t>
-  </si>
-  <si>
-    <t>Lookup table incomplete</t>
-  </si>
-  <si>
-    <t>Elizabeth advised this should be left blank/null</t>
-  </si>
-  <si>
-    <t>finance_invoice_non_ad</t>
+exclude_values = {"col": "Invoice_Type", "values": ["AD"]}
+recent_or_open_invoices={"date_col": "Create", "tax_year_from": 2019}
+greater_than = {"col": "Amount", "value": 0}</t>
   </si>
   <si>
     <t>first_x_chars = {"col": "Invoice No", "result_col": "Invoice_Type", "num": 2}
-exclude_values = {"col": "Invoice_Type", "values": ["AD"]}</t>
-  </si>
-  <si>
-    <t>AD</t>
-  </si>
-  <si>
-    <t>start_of_tax_year</t>
-  </si>
-  <si>
-    <t>end_of_tax_year</t>
+Invoice_Type = "AD"
+recent_or_open_invoices={"date_col": "Create", "tax_year_from": 2019}
+greater_than = {"col": "Amount", "value": 0}</t>
+  </si>
+  <si>
+    <t>Case, Invoice No, Amount, Create</t>
   </si>
 </sst>
 </file>
@@ -624,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D765A69-DF19-B84F-A530-22008AF977F3}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -639,74 +637,74 @@
   <sheetData>
     <row r="1" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="8" t="s">
+    </row>
+    <row r="2" spans="1:8" s="9" customFormat="1" ht="112" x14ac:dyDescent="0.15">
+      <c r="A2" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" s="9" customFormat="1" ht="56" x14ac:dyDescent="0.15">
-      <c r="A2" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="9" t="s">
+      <c r="F2" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="9" customFormat="1" ht="126" x14ac:dyDescent="0.15">
+      <c r="A3" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="9" customFormat="1" ht="70" x14ac:dyDescent="0.15">
-      <c r="A3" s="10" t="s">
+      <c r="E3" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>79</v>
-      </c>
       <c r="H3" s="10" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
@@ -723,7 +721,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -796,10 +794,10 @@
     </row>
     <row r="2" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>38</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>39</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>16</v>
@@ -811,7 +809,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G2" s="9"/>
       <c r="O2" s="3" t="s">
@@ -823,13 +821,13 @@
     </row>
     <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>39</v>
-      </c>
       <c r="C3" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>17</v>
@@ -843,18 +841,18 @@
         <v>18</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>39</v>
-      </c>
       <c r="C4" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>17</v>
@@ -864,28 +862,28 @@
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="13" t="s">
         <v>18</v>
       </c>
       <c r="P4" s="14" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>39</v>
-      </c>
       <c r="C5" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="9" t="b">
         <v>0</v>
@@ -893,7 +891,7 @@
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="M5" s="14" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="13" t="s">
@@ -902,16 +900,16 @@
     </row>
     <row r="6" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>39</v>
-      </c>
       <c r="C6" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" s="9" t="b">
         <v>0</v>
@@ -919,11 +917,11 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I6" s="11"/>
       <c r="J6" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="O6" s="13" t="s">
         <v>18</v>
@@ -931,13 +929,13 @@
     </row>
     <row r="7" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>39</v>
-      </c>
       <c r="C7" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>20</v>
@@ -948,10 +946,10 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="M7" s="2"/>
       <c r="O7" s="13" t="s">
@@ -960,13 +958,13 @@
     </row>
     <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>39</v>
-      </c>
       <c r="C8" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>20</v>
@@ -977,14 +975,14 @@
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I8" s="11"/>
       <c r="J8" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="L8" s="2"/>
       <c r="O8" s="13" t="s">
@@ -993,13 +991,13 @@
     </row>
     <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>39</v>
-      </c>
       <c r="C9" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>17</v>
@@ -1010,13 +1008,13 @@
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O9" s="12" t="s">
         <v>18</v>
@@ -1024,16 +1022,16 @@
     </row>
     <row r="10" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>39</v>
-      </c>
       <c r="C10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>23</v>
       </c>
       <c r="E10" s="9" t="b">
         <v>0</v>
@@ -1041,30 +1039,28 @@
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="O10" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="P10" s="14" t="s">
-        <v>76</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="P10" s="14"/>
     </row>
     <row r="11" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>39</v>
-      </c>
       <c r="C11" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>17</v>
@@ -1074,24 +1070,24 @@
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O11" s="15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="P11" s="14" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>39</v>
-      </c>
       <c r="C12" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>20</v>
@@ -1102,21 +1098,21 @@
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="O12" s="15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="P12" s="14" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>39</v>
-      </c>
       <c r="C13" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>17</v>
@@ -1127,21 +1123,21 @@
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="O13" s="15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="P13" s="14" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>39</v>
-      </c>
       <c r="C14" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>20</v>
@@ -1152,10 +1148,10 @@
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O14" s="2" t="s">
         <v>18</v>
@@ -1163,16 +1159,16 @@
     </row>
     <row r="15" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>39</v>
-      </c>
       <c r="C15" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E15" s="9" t="b">
         <v>0</v>
@@ -1180,7 +1176,7 @@
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="M15" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O15" s="15" t="s">
         <v>18</v>
@@ -2591,9 +2587,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B46E64-4858-2243-9F40-616107ECC251}">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomLeft" activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2666,10 +2662,10 @@
     </row>
     <row r="2" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>38</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>39</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>16</v>
@@ -2681,7 +2677,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G2" s="9"/>
       <c r="O2" s="3" t="s">
@@ -2693,13 +2689,13 @@
     </row>
     <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>39</v>
-      </c>
       <c r="C3" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>17</v>
@@ -2713,18 +2709,18 @@
         <v>18</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>39</v>
-      </c>
       <c r="C4" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>17</v>
@@ -2734,28 +2730,28 @@
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="13" t="s">
         <v>18</v>
       </c>
       <c r="P4" s="14" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>39</v>
-      </c>
       <c r="C5" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="9" t="b">
         <v>0</v>
@@ -2763,13 +2759,13 @@
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="H5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="13" t="s">
@@ -2778,16 +2774,16 @@
     </row>
     <row r="6" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>39</v>
-      </c>
       <c r="C6" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" s="9" t="b">
         <v>0</v>
@@ -2795,11 +2791,11 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I6" s="11"/>
       <c r="J6" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="O6" s="13" t="s">
         <v>18</v>
@@ -2807,13 +2803,13 @@
     </row>
     <row r="7" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>39</v>
-      </c>
       <c r="C7" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>20</v>
@@ -2824,13 +2820,13 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="M7" s="2"/>
       <c r="O7" s="13" t="s">
@@ -2839,13 +2835,13 @@
     </row>
     <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>39</v>
-      </c>
       <c r="C8" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>20</v>
@@ -2856,14 +2852,14 @@
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I8" s="11"/>
       <c r="J8" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="L8" s="2"/>
       <c r="O8" s="13" t="s">
@@ -2872,13 +2868,13 @@
     </row>
     <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>39</v>
-      </c>
       <c r="C9" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>17</v>
@@ -2889,13 +2885,13 @@
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O9" s="12" t="s">
         <v>18</v>
@@ -2903,16 +2899,16 @@
     </row>
     <row r="10" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>39</v>
-      </c>
       <c r="C10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>23</v>
       </c>
       <c r="E10" s="9" t="b">
         <v>0</v>
@@ -2920,30 +2916,28 @@
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="O10" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="P10" s="14" t="s">
-        <v>76</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="P10" s="14"/>
     </row>
     <row r="11" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>39</v>
-      </c>
       <c r="C11" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>17</v>
@@ -2953,24 +2947,24 @@
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O11" s="15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="P11" s="14" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>39</v>
-      </c>
       <c r="C12" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>20</v>
@@ -2981,21 +2975,21 @@
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="O12" s="15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="P12" s="14" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>39</v>
-      </c>
       <c r="C13" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>17</v>
@@ -3006,21 +3000,21 @@
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="O13" s="15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="P13" s="14" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>39</v>
-      </c>
       <c r="C14" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>20</v>
@@ -3031,10 +3025,10 @@
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O14" s="2" t="s">
         <v>18</v>
@@ -3042,16 +3036,16 @@
     </row>
     <row r="15" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>39</v>
-      </c>
       <c r="C15" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E15" s="9" t="b">
         <v>0</v>
@@ -3059,7 +3053,7 @@
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="M15" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O15" s="15" t="s">
         <v>18</v>
@@ -4474,7 +4468,7 @@
   <dimension ref="A1:E998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4485,42 +4479,42 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B4" s="3"/>
       <c r="E4" s="7"/>

</xml_diff>